<commit_message>
new changes and cooection of master screen
</commit_message>
<xml_diff>
--- a/SMSApplication/bin/Debug/Templates/Staff Master Template Import.xlsx
+++ b/SMSApplication/bin/Debug/Templates/Staff Master Template Import.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>S.No.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Blood Group</t>
   </si>
@@ -46,9 +43,6 @@
   </si>
   <si>
     <t>Pincode</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>Staff Name</t>
@@ -417,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
@@ -443,27 +437,27 @@
     <col min="17" max="17" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -477,14 +471,9 @@
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:11">
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
   </sheetData>

</xml_diff>